<commit_message>
Add empty row to Query
</commit_message>
<xml_diff>
--- a/src/test/resources/Query/QueryTemplate.xlsx
+++ b/src/test/resources/Query/QueryTemplate.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="6360" yWindow="1880" windowWidth="25120" windowHeight="18540" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>PatientName</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>123456</t>
+  </si>
+  <si>
+    <t>Test3</t>
   </si>
 </sst>
 </file>
@@ -448,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -540,6 +543,14 @@
         <v>16</v>
       </c>
     </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>